<commit_message>
Changed weightings of individual and communal keywords xlsx files
</commit_message>
<xml_diff>
--- a/data/communal_keywords.xlsx
+++ b/data/communal_keywords.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Keyword</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>Mentor</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>Husband</t>
+  </si>
+  <si>
+    <t>Wife</t>
   </si>
 </sst>
 </file>
@@ -455,7 +464,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3">
@@ -839,6 +848,38 @@
         <v>50</v>
       </c>
       <c r="B50" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="1">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>